<commit_message>
Built site for MassWateR: 2.0.2.9000@30aa993
</commit_message>
<xml_diff>
--- a/ExampleDQOAccuracy.xlsx
+++ b/ExampleDQOAccuracy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Example input files\Official Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BB4B32-1A70-4433-9D48-E59EBFE69CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92362BF2-DFB3-4BE9-A1A0-287474DE944F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="74">
   <si>
     <t>Parameter</t>
   </si>
@@ -103,6 +103,12 @@
     <t>E.coli</t>
   </si>
   <si>
+    <t>&lt;50</t>
+  </si>
+  <si>
+    <t>&gt;=50</t>
+  </si>
+  <si>
     <t>&lt;=log30%</t>
   </si>
   <si>
@@ -199,6 +205,9 @@
     <t>Enter the spike or calibration check data quality objective.  This will be used for Lab Spikes and Instrument Calibration Checks.  This can also be used for performance evaluation samples, such as outside standards that are used to assess lab analytical accuracy.</t>
   </si>
   <si>
+    <t>Template updated 12/7/22</t>
+  </si>
+  <si>
     <t>Water Temp</t>
   </si>
   <si>
@@ -241,16 +250,13 @@
     <t>MPN/100ml</t>
   </si>
   <si>
-    <t>&lt;50</t>
-  </si>
-  <si>
     <t>&lt; log30%</t>
   </si>
   <si>
-    <t>&gt;=50</t>
-  </si>
-  <si>
     <t>&lt; log20%</t>
+  </si>
+  <si>
+    <t>Samples updated 1/8/23</t>
   </si>
 </sst>
 </file>
@@ -260,7 +266,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +294,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -362,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -420,6 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,25 +818,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973C1027-43ED-409D-9786-38F45BEFD8D3}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12:XFD13"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="5" customWidth="1"/>
-    <col min="3" max="4" width="8.81640625" style="5" customWidth="1"/>
-    <col min="5" max="10" width="12.26953125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="5" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="5" customWidth="1"/>
+    <col min="5" max="10" width="12.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -854,12 +868,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
@@ -871,10 +885,10 @@
         <v>16</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>15</v>
@@ -883,15 +897,15 @@
         <v>15</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>15</v>
@@ -903,27 +917,27 @@
         <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
@@ -935,7 +949,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>15</v>
@@ -950,12 +964,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>15</v>
@@ -967,7 +981,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>15</v>
@@ -982,12 +996,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>15</v>
@@ -996,30 +1010,30 @@
         <v>15</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>15</v>
@@ -1028,30 +1042,30 @@
         <v>10000</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5">
         <v>0.01</v>
@@ -1063,10 +1077,10 @@
         <v>12</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>7</v>
@@ -1075,15 +1089,15 @@
         <v>7</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5">
         <v>0.01</v>
@@ -1095,10 +1109,10 @@
         <v>13</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>7</v>
@@ -1107,15 +1121,15 @@
         <v>7</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5">
         <v>0.05</v>
@@ -1127,10 +1141,10 @@
         <v>16</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>7</v>
@@ -1139,15 +1153,15 @@
         <v>7</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5">
         <v>0.1</v>
@@ -1159,10 +1173,10 @@
         <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>7</v>
@@ -1171,15 +1185,15 @@
         <v>7</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -1188,13 +1202,13 @@
         <v>15</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>7</v>
@@ -1206,12 +1220,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -1220,13 +1234,13 @@
         <v>15</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>7</v>
@@ -1245,204 +1259,210 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83CEA30-4E88-458A-AFF2-D4098CA8390C}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" customWidth="1"/>
-    <col min="2" max="2" width="96.453125" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="96.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C8" s="13">
         <v>0.1</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C9" s="12">
         <v>1500</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>